<commit_message>
Fixed Deposit 15 test cases.
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4742-SUBMITFDS01JAN2015(DEPOPRD12MNTH)-ADDCHRGE-APRACT01FEB2015.xlsx
+++ b/Mifos Automation Excels/Client/4742-SUBMITFDS01JAN2015(DEPOPRD12MNTH)-ADDCHRGE-APRACT01FEB2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="NewFDInput" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
   <si>
     <t>clickonmorebutton</t>
   </si>
@@ -61,21 +61,6 @@
     <t>save</t>
   </si>
   <si>
-    <t>clickonmorebutton1</t>
-  </si>
-  <si>
-    <t>FDAddChargeButton</t>
-  </si>
-  <si>
-    <t>charges</t>
-  </si>
-  <si>
-    <t>Saving Charge-Saving Activation-Flat(US Dollar)</t>
-  </si>
-  <si>
-    <t>DueForCollectionOn</t>
-  </si>
-  <si>
     <t>Submitbutton1</t>
   </si>
   <si>
@@ -187,9 +172,6 @@
     <t>fee</t>
   </si>
   <si>
-    <t>Savings Activation</t>
-  </si>
-  <si>
     <t>Flat</t>
   </si>
   <si>
@@ -212,13 +194,37 @@
   </si>
   <si>
     <t>Saving Charge-Specified due date-Flat</t>
+  </si>
+  <si>
+    <t>Saving Charge-Specified due date-Flat,$</t>
+  </si>
+  <si>
+    <t>Specified due date</t>
+  </si>
+  <si>
+    <t>Interest earned</t>
+  </si>
+  <si>
+    <t>Interest posted</t>
+  </si>
+  <si>
+    <t>$ 37.05</t>
+  </si>
+  <si>
+    <t>Savingclickonplusbutton</t>
+  </si>
+  <si>
+    <t>Savinginsertdate</t>
+  </si>
+  <si>
+    <t>clickonFDCharge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +244,14 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -269,10 +283,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -286,17 +301,21 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -637,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,97 +726,81 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>64</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="B10" s="3">
+        <v>42005</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="3">
-        <v>42005</v>
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>42005</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="3">
-        <v>42005</v>
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="B16" s="3">
+        <v>42005</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="3">
-        <v>42005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -808,45 +811,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6">
         <v>42005</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5">
         <v>3</v>
@@ -854,17 +857,29 @@
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B4" s="6">
         <v>42370</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -879,64 +894,67 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6">
-        <v>42005</v>
+        <v>42036</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D2" s="5">
         <v>100</v>
       </c>
       <c r="E2" s="5"/>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>4900</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="B3" s="6">
         <v>42005</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>5000</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>5000</v>
       </c>
     </row>
@@ -947,67 +965,68 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
+      <c r="J1" s="7"/>
+      <c r="K1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="O1" s="7"/>
+      <c r="P1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8" t="s">
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D2" s="5"/>
-      <c r="E2" t="s">
-        <v>54</v>
+      <c r="E2" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="6">
@@ -1015,25 +1034,26 @@
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1042,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,26 +1075,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
+      <c r="A2" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>60</v>
+      <c r="A3" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B3" s="3">
         <v>42036</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>